<commit_message>
complete testing full_obs for use in ccanada
</commit_message>
<xml_diff>
--- a/pendulum/full_obs_pendulum/full_obs_raw_data.xlsx
+++ b/pendulum/full_obs_pendulum/full_obs_raw_data.xlsx
@@ -8,30 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/full_obs_pendulum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8AD1C6AB-4E94-0640-91BB-65DC915CDE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B121BC7F-F1C4-674E-8AFF-38E18721BB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15680" xr2:uid="{0B69977A-7230-EF48-AC0B-2C9BBEA88D25}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -389,10 +373,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03450918-53B1-6D4E-8292-8F07E8D373EF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>

<commit_message>
create main with func to be run on ccanada
</commit_message>
<xml_diff>
--- a/pendulum/full_obs_pendulum/full_obs_raw_data.xlsx
+++ b/pendulum/full_obs_pendulum/full_obs_raw_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/full_obs_pendulum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B121BC7F-F1C4-674E-8AFF-38E18721BB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4D4CB1-D493-F540-A74B-38AF96E87082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -377,7 +377,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix write to excel
</commit_message>
<xml_diff>
--- a/pendulum/full_obs_pendulum/full_obs_raw_data.xlsx
+++ b/pendulum/full_obs_pendulum/full_obs_raw_data.xlsx
@@ -1,34 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/full_obs_pendulum/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4516B3C-263B-2440-8592-14176CBA0BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15680" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="9.81" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>empty</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,80 +59,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,90 +373,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>empty</t>
-        </is>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>ind</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>fitness</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>conditional(add(y, add(y, y)), add(add(y, y), add(y, add(add(add(vel, x), conditional(x, conditional(add(conditional(y, conditional(conditional(conditional(x, x), add(x, x)), add(add(conditional(add(conditional(x, vel), add(x, y)), add(add(add(vel, x), x), add(x, x))), add(vel, x)), vel))), add(add(add(conditional(y, vel), x), conditional(vel, add(x, y))), add(y, add(x, add(conditional(add(x, vel), add(y, y)), add(y, y)))))), add(add(y, conditional(conditional(y, x), conditional(x, vel))), add(add(conditional(add(x, y), add(y, vel)), x), x))))), add(add(x, add(x, x)), add(x, x))))))</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>-98</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>ind</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>fitness</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>conditional(conditional(add(x, x), conditional(vel, x)), add(conditional(vel, vel), conditional(add(add(vel, x), add(y, y)), y)))</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>-2132</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
clean up full obs code
</commit_message>
<xml_diff>
--- a/pendulum/full_obs_pendulum/full_obs_raw_data.xlsx
+++ b/pendulum/full_obs_pendulum/full_obs_raw_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15680" tabRatio="600" firstSheet="0" activeTab="8" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15680" tabRatio="600" firstSheet="0" activeTab="9" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="15" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="16" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="17" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="1" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -452,6 +453,47 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ind</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>fitness</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>conditional(conditional(y, y), add(vel, x))</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-317</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
clean up full_obs for use with modules dir
</commit_message>
<xml_diff>
--- a/pendulum/full_obs_pendulum/full_obs_raw_data.xlsx
+++ b/pendulum/full_obs_pendulum/full_obs_raw_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15680" tabRatio="600" firstSheet="0" activeTab="9" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15680" tabRatio="600" firstSheet="0" activeTab="10" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="16" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="17" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="1" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="2" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -459,6 +460,57 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ind</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>fitness</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>conditional(conditional(y, y), add(vel, x))</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-317</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>add(add(add(y, x), conditional(y, y)), conditional(conditional(y, x), conditional(y, y)))</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-1905</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -482,11 +534,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>conditional(conditional(y, y), add(vel, x))</t>
+          <t>conditional(conditional(conditional(x, vel), add(y, vel)), conditional(vel, vel))</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-317</v>
+        <v>-854</v>
       </c>
     </row>
   </sheetData>

</xml_diff>